<commit_message>
rRNA analysis alpha version
</commit_message>
<xml_diff>
--- a/huenRNA/analysis/rRNA-mapping-strategies.xlsx
+++ b/huenRNA/analysis/rRNA-mapping-strategies.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuanhua/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuanhua/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8A918D-FCD1-FF41-913C-B98C4CC8D9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9ECA6C-6FC3-CE40-9182-1700614CF3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{867EF11F-7B90-AE42-B0C0-85E4784E00DF}"/>
+    <workbookView xWindow="3960" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="1" xr2:uid="{867EF11F-7B90-AE42-B0C0-85E4784E00DF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="map2rRNA" sheetId="1" r:id="rId1"/>
+    <sheet name="map2mRNA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="61">
   <si>
     <t xml:space="preserve">                                    UNIQUE READS:</t>
   </si>
@@ -196,6 +196,30 @@
   </si>
   <si>
     <t>45S without padding (0.66 mapped length)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Sep 07 07:24:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Sep 07 07:24:49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Sep 07 07:29:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Sep 07 19:00:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Sep 07 19:01:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Sep 07 19:05:46</t>
+  </si>
+  <si>
+    <t>after ribodetector</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> after STAR (45S no padding)</t>
   </si>
 </sst>
 </file>
@@ -244,13 +268,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC77539-876B-EA47-A42F-AC2130093D99}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1124,7 +1147,7 @@
       <c r="D26" s="2">
         <v>3.8800000000000001E-2</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="1">
         <v>1.09E-2</v>
       </c>
       <c r="J26" s="4" t="s">
@@ -1384,53 +1407,426 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF666FC-64C7-2D4F-AE71-265599A0423F}">
-  <dimension ref="B10:C37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="1"/>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>171.96</v>
+      </c>
+      <c r="D5">
+        <v>225.37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>14282416</v>
+      </c>
+      <c r="D7" s="3">
+        <v>17653730</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>300</v>
+      </c>
+      <c r="D8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8381980</v>
+      </c>
       <c r="C10" s="1"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="1"/>
+      <c r="D10">
+        <v>9342811</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.58689999999999998</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.5292</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3">
+        <v>279.13</v>
+      </c>
+      <c r="D12">
+        <v>281.38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>4532853</v>
+      </c>
+      <c r="D13">
+        <v>4620367</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>4462400</v>
+      </c>
+      <c r="D14">
+        <v>4464898</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>4478677</v>
+      </c>
+      <c r="D15">
+        <v>4503252</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>35068</v>
+      </c>
+      <c r="D16">
+        <v>36410</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>4536</v>
+      </c>
+      <c r="D17">
+        <v>4614</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>14572</v>
+      </c>
       <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="1"/>
+      <c r="D18">
+        <v>76091</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3.3E-3</v>
+      </c>
       <c r="C19" s="1"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="1"/>
+      <c r="D19" s="1">
+        <v>3.3999999999999998E-3</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>1.3</v>
+      </c>
       <c r="C21" s="1"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="1"/>
+      <c r="D21">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>1.86</v>
+      </c>
+      <c r="D23">
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>4616478</v>
+      </c>
       <c r="C25" s="1"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B27" s="1"/>
+      <c r="D25">
+        <v>7068350</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.32319999999999999</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.40039999999999998</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>289769</v>
+      </c>
       <c r="C27" s="1"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B30" s="1"/>
+      <c r="D27">
+        <v>227670</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2.0299999999999999E-2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1.29E-2</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
       <c r="C30" s="1"/>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B32" s="1"/>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>504954</v>
+      </c>
       <c r="C32" s="1"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B34" s="1"/>
+      <c r="D32">
+        <v>415662</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="1">
+        <v>3.5400000000000001E-2</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2.35E-2</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>489235</v>
+      </c>
       <c r="C34" s="1"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
+      <c r="D34">
+        <v>599237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="1">
+        <v>3.4299999999999997E-2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>3.39E-2</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
       <c r="C37" s="1"/>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="J38" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>